<commit_message>
Imprimiendo resultados en boxplots
</commit_message>
<xml_diff>
--- a/PIA/Tic Tac Toe/datos_rondas.xlsx
+++ b/PIA/Tic Tac Toe/datos_rondas.xlsx
@@ -1,23 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amigo\Documents\Documentos FCFM\6to Semestre\Inteligencia Artificial\PIA - Equipo 6\Codigo\PIA_Inteligencia_Artificial\PIA\Tic Tac Toe\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFABFE3D-4489-477C-97BA-39BF21B32E66}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="6">
-  <si>
-    <t>Round</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="5">
   <si>
     <t>Min_time</t>
   </si>
@@ -37,8 +40,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -101,11 +104,19 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -147,7 +158,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -179,9 +190,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -213,6 +242,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -388,14 +435,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -405,11 +452,8 @@
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -417,353 +461,290 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>0.5802569389343262</v>
-      </c>
-      <c r="E2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+        <v>0.58025693893432617</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>6.18106484413147</v>
-      </c>
-      <c r="E3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+        <v>6.1810648441314697</v>
+      </c>
+      <c r="D3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>0.009994268417358398</v>
-      </c>
-      <c r="E4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+        <v>9.9942684173583984E-3</v>
+      </c>
+      <c r="D4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5">
-        <v>3</v>
+        <v>9.7937583923339844E-3</v>
       </c>
       <c r="C5">
-        <v>0.009793758392333984</v>
-      </c>
-      <c r="D5">
-        <v>0.009999275207519531</v>
-      </c>
-      <c r="E5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+        <v>9.9992752075195313E-3</v>
+      </c>
+      <c r="D5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>0.02975153923034668</v>
-      </c>
-      <c r="E6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
+        <v>2.975153923034668E-2</v>
+      </c>
+      <c r="D6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7">
-        <v>0.7696104049682617</v>
-      </c>
-      <c r="E7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
+        <v>0.76961040496826172</v>
+      </c>
+      <c r="D7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <v>0.7100636959075928</v>
-      </c>
-      <c r="E8" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
+        <v>0.71006369590759277</v>
+      </c>
+      <c r="D8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="B9">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="C9">
         <v>0</v>
       </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
+      <c r="D9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="B10">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C10">
-        <v>0</v>
-      </c>
-      <c r="D10">
-        <v>0.02998447418212891</v>
-      </c>
-      <c r="E10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
+        <v>2.998447418212891E-2</v>
+      </c>
+      <c r="D10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
       <c r="B11">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="C11">
-        <v>0</v>
-      </c>
-      <c r="D11">
-        <v>0.01999258995056152</v>
-      </c>
-      <c r="E11" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
+        <v>1.999258995056152E-2</v>
+      </c>
+      <c r="D11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>10</v>
       </c>
       <c r="B12">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C12">
-        <v>0</v>
-      </c>
-      <c r="D12">
         <v>0.920074462890625</v>
       </c>
-      <c r="E12" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
+      <c r="D12" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
       <c r="B13">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="C13">
-        <v>0</v>
-      </c>
-      <c r="D13">
-        <v>0.6303656101226807</v>
-      </c>
-      <c r="E13" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
+        <v>0.63036561012268066</v>
+      </c>
+      <c r="D13" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>12</v>
       </c>
       <c r="B14">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="C14">
-        <v>0</v>
-      </c>
-      <c r="D14">
-        <v>0.7298352718353271</v>
-      </c>
-      <c r="E14" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
+        <v>0.72983527183532715</v>
+      </c>
+      <c r="D14" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>13</v>
       </c>
       <c r="B15">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="C15">
-        <v>0</v>
-      </c>
-      <c r="D15">
-        <v>0.678382396697998</v>
-      </c>
-      <c r="E15" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
+        <v>0.67838239669799805</v>
+      </c>
+      <c r="D15" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>14</v>
       </c>
       <c r="B16">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="C16">
-        <v>0</v>
-      </c>
-      <c r="D16">
-        <v>0.02977871894836426</v>
-      </c>
-      <c r="E16" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
+        <v>2.9778718948364261E-2</v>
+      </c>
+      <c r="D16" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>15</v>
       </c>
       <c r="B17">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="C17">
         <v>0</v>
       </c>
-      <c r="D17">
-        <v>0</v>
-      </c>
-      <c r="E17" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
+      <c r="D17" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>16</v>
       </c>
       <c r="B18">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="C18">
-        <v>0</v>
-      </c>
-      <c r="D18">
-        <v>0.01975727081298828</v>
-      </c>
-      <c r="E18" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
+        <v>1.9757270812988281E-2</v>
+      </c>
+      <c r="D18" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>17</v>
       </c>
       <c r="B19">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="C19">
-        <v>0</v>
-      </c>
-      <c r="D19">
-        <v>6.021164417266846</v>
-      </c>
-      <c r="E19" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
+        <v>6.0211644172668457</v>
+      </c>
+      <c r="D19" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>18</v>
       </c>
       <c r="B20">
-        <v>18</v>
+        <v>9.9778175354003906E-4</v>
       </c>
       <c r="C20">
-        <v>0.0009977817535400391</v>
-      </c>
-      <c r="D20">
-        <v>0.6101398468017578</v>
-      </c>
-      <c r="E20" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
+        <v>0.61013984680175781</v>
+      </c>
+      <c r="D20" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>19</v>
       </c>
       <c r="B21">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="C21">
-        <v>0</v>
-      </c>
-      <c r="D21">
-        <v>0.009967803955078125</v>
-      </c>
-      <c r="E21" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
+        <v>9.967803955078125E-3</v>
+      </c>
+      <c r="D21" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>20</v>
       </c>
       <c r="B22">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C22">
-        <v>0</v>
-      </c>
-      <c r="D22">
-        <v>6.071532249450684</v>
-      </c>
-      <c r="E22" t="s">
-        <v>4</v>
+        <v>6.0715322494506836</v>
+      </c>
+      <c r="D22" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>